<commit_message>
Added Class Level initialization for Driver Launch&Quit
</commit_message>
<xml_diff>
--- a/src/main/java/resources/testData/ExcelTestData.xlsx
+++ b/src/main/java/resources/testData/ExcelTestData.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nnagaraju/Documents/Automation/itppm_test_automation/src/main/java/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD41F75-BF90-D844-A78E-98EDB5932FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CE3688-28CB-A342-A919-6DD3D630ECC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="1100" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{31E1E056-7656-F64C-88F5-A8D8A3278946}"/>
   </bookViews>
   <sheets>
     <sheet name="TC001" sheetId="1" r:id="rId1"/>
     <sheet name="TC002" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -484,7 +483,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,16 +504,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB29D39-C323-B24A-9661-4842A5A8CC7C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>